<commit_message>
ahora sube los datos de retiros a una base de datos
</commit_message>
<xml_diff>
--- a/static/tmp/planificacion.xlsx
+++ b/static/tmp/planificacion.xlsx
@@ -1,37 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Trackers</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>fechas</t>
+  </si>
+  <si>
+    <t>end_time</t>
+  </si>
+  <si>
+    <t>start_to_end_time</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +72,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,52 +388,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Trackers</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>fechas</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>start_to_end_time</t>
-        </is>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
contempla a quien darle viajes segun tipo de conductor
</commit_message>
<xml_diff>
--- a/static/tmp/planificacion.xlsx
+++ b/static/tmp/planificacion.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="244">
   <si>
     <t>id</t>
   </si>
@@ -34,28 +34,154 @@
     <t>start_to_end_time</t>
   </si>
   <si>
+    <t>('FRANCISCO VIDAL L', 'ASOCIADO', 1, 1, '19.403.547-0')</t>
+  </si>
+  <si>
+    <t>('JOSE VIDAL J', 'ASOCIADO', 1, 1, '8.780.104-7')</t>
+  </si>
+  <si>
+    <t>('JUAN VICENCIO N', 'PROPIO', 0, 1, '15.095.552-1')</t>
+  </si>
+  <si>
+    <t>('CARLOS TAPIA', 'ASOCIADO', 1, 1, '9.262.912-0')</t>
+  </si>
+  <si>
+    <t>('EDUARDO ROMAN O', 'PROPIO', 0, 1, '11.946.072-7')</t>
+  </si>
+  <si>
+    <t>('JOSE SANTIS S', 'PROPIO', 0, 1, '15.872.022-1')</t>
+  </si>
+  <si>
+    <t>('AURELIO ARÉVALO G', 'ASOCIADO', 1, 1, '13.196.601-6')</t>
+  </si>
+  <si>
+    <t>('MARCO CATALDO C', 'TERCERO', 2, 0, '16.777.267-6')</t>
+  </si>
+  <si>
+    <t>('ADOLFO CORVALAN P', 'PROPIO', 0, 1, '19.758.425-4')</t>
+  </si>
+  <si>
+    <t>('CARLOS AREVALO M', 'PROPIO', 0, 1, '17.149.048-0')</t>
+  </si>
+  <si>
+    <t>('JUAN BERNACHEA', 'ASOCIADO', 1, 1, '7.741.876-8')</t>
+  </si>
+  <si>
+    <t>('SERGIO VEGA V', 'PROPIO', 0, 1, '18.122.272-7')</t>
+  </si>
+  <si>
+    <t>('GABRIEL PARRA C', 'ASOCIADO', 1, 1, '18.759.852-4')</t>
+  </si>
+  <si>
+    <t>('ABELARDO CONSTANTE T', 'PROPIO', 0, 1, '28.036.888-1')</t>
+  </si>
+  <si>
+    <t>('DANIEL BEJARANO H', 'PROPIO', 0, 1, '27.886.201-1')</t>
+  </si>
+  <si>
+    <t>('NATALY GONZALEZ M', 'ASOCIADO', 1, 1, '17.444.914-7')</t>
+  </si>
+  <si>
+    <t>('MAURICIO MAULEN', 'ASOCIADO', 1, 1, '11.275.919-0')</t>
+  </si>
+  <si>
+    <t>('LUIS REYES P', 'ASOCIADO', 1, 1, '8.298.532-8')</t>
+  </si>
+  <si>
+    <t>('DANIEL  L', 'ASOCIADO', 1, 1, '15.873.188-6')</t>
+  </si>
+  <si>
+    <t>('PATRICIO CARREÑO B', 'PROPIO', 0, 1, '15.348.250-0')</t>
+  </si>
+  <si>
+    <t>('ANGEL CARREÑO', 'ASOCIADO', 1, 1, '14.003.333-2')</t>
+  </si>
+  <si>
+    <t>('JHONNY SEPULVEDA', 'ASOCIADO', 1, 1, '16.130.818-8')</t>
+  </si>
+  <si>
+    <t>('FRANCISCO GARCIA D', 'PROPIO', 0, 1, '18.228.515-3')</t>
+  </si>
+  <si>
+    <t>('JORGE ALFARO H', 'ASOCIADO', 1, 1, '16.758.352-0')</t>
+  </si>
+  <si>
+    <t>('JOSE GONZALEZ B', 'ASOCIADO', 1, 1, '9.813.300-3')</t>
+  </si>
+  <si>
+    <t>('RODRIGO RIQUELME N', 'ASOCIADO', 1, 1, '13.767.617-6')</t>
+  </si>
+  <si>
+    <t>('EDUARDO MARAMBIO A', 'ASOCIADO', 1, 1, '18.760.890-2')</t>
+  </si>
+  <si>
+    <t>('BETHI PROAÑO R', 'PORTEADOR', 0, 1, '28.060.670-7')</t>
+  </si>
+  <si>
+    <t>('MANUEL VIDAL L', 'ASOCIADO', 1, 1, '16.311.233-7')</t>
+  </si>
+  <si>
+    <t>('SAMUEL FAUNDEZ J', 'ASOCIADO', 1, 1, '16.265.186-2')</t>
+  </si>
+  <si>
+    <t>('ANGEL FLORES H', 'ASOCIADO', 1, 1, '16.668.125-1')</t>
+  </si>
+  <si>
+    <t>('JOSE REYES', 'ASOCIADO', 1, 1, '14.003.298-0')</t>
+  </si>
+  <si>
+    <t>('JOSE SANCHEZ', 'ASOCIADO', 1, 1, '27.742.628-5')</t>
+  </si>
+  <si>
+    <t>('MAURICIO URBINA S', 'PROPIO', 0, 1, '11.630.504-6')</t>
+  </si>
+  <si>
+    <t>('CAMILO PLAZA G', 'ASOCIADO', 1, 1, '15.401.957-K')</t>
+  </si>
+  <si>
+    <t>('ANDY BETANCOURT H', 'PROPIO', 0, 1, '16.300.244-2')</t>
+  </si>
+  <si>
+    <t>('IVAN PARRA C', 'ASOCIADO', 1, 1, '19.143.325-4')</t>
+  </si>
+  <si>
     <t>('OSWALDO ESCALONA A', 'PORTEADOR', 0, 1, '27.643.631-7')</t>
   </si>
   <si>
-    <t>('RODRIGO RIQUELME N', 'ASOCIADO', 1, 1, '13.767.617-6')</t>
-  </si>
-  <si>
-    <t>('JOSE SANTIS S', 'PROPIO', 0, 1, '15.872.022-1')</t>
-  </si>
-  <si>
-    <t>('EDUARDO MARAMBIO A', 'ASOCIADO', 1, 1, '18.760.890-2')</t>
-  </si>
-  <si>
-    <t>('PATRICIO CARREÑO B', 'PROPIO', 0, 1, '15.348.250-0')</t>
-  </si>
-  <si>
-    <t>('JUAN BERNACHEA', 'ASOCIADO', 1, 1, '7.741.876-8')</t>
-  </si>
-  <si>
-    <t>('ADOLFO CORVALAN P', 'PROPIO', 0, 1, '19.758.425-4')</t>
-  </si>
-  <si>
-    <t>('DANIEL  L', 'ASOCIADO', 1, 1, '15.873.188-6')</t>
+    <t>('CRISTIAN MUÑOZ S', 'ASOCIADO', 1, 1, '13.196.333-5')</t>
+  </si>
+  <si>
+    <t>('Luis Arevalo M', 'ASOCIADO', 1, 1, '16.529.122-0')</t>
+  </si>
+  <si>
+    <t>('GUILLERMO GARAY', 'ASOCIADO', 1, 1, '15.648.946-8')</t>
+  </si>
+  <si>
+    <t>('Luis Olea V', 'PROPIO', 0, 1, '16.491.628-6')</t>
+  </si>
+  <si>
+    <t>('DOMINGO LLANOS', 'ASOCIADO', 1, 1, '10.767.591-4')</t>
+  </si>
+  <si>
+    <t>('MARCO BERNACHEA A', 'ASOCIADO', 1, 1, '13.665.862-K')</t>
+  </si>
+  <si>
+    <t>('RICARDO GONZALEZ L', 'ASOCIADO', 1, 1, '7.614.149-5')</t>
+  </si>
+  <si>
+    <t>('MAURICIO RIVAS R', 'ASOCIADO', 1, 1, '18.448.238-K')</t>
+  </si>
+  <si>
+    <t>('Nelson Gallardo R', 'PROPIO', 0, 1, '11.388.715-K')</t>
+  </si>
+  <si>
+    <t>('OWEN AGUILAR G', 'ASOCIADO', 1, 1, '15.873.472-9')</t>
+  </si>
+  <si>
+    <t>('CRISTIAN REAL M', 'PORTEADOR', 0, 1, '16.642.093-8')</t>
+  </si>
+  <si>
+    <t>('CARLOS PONCE A', 'PROPIO', 0, 1, '14.555.433-0')</t>
   </si>
   <si>
     <t>('RODRIGO  I', 'PROPIO', 0, 1, '10.355.521-3')</t>
@@ -64,565 +190,562 @@
     <t>('Rene Vives H', 'PROPIO', 0, 1, '10.813.755-K')</t>
   </si>
   <si>
-    <t>('AURELIO ARÉVALO G', 'ASOCIADO', 1, 1, '13.196.601-6')</t>
-  </si>
-  <si>
-    <t>('FRANCISCO VIDAL L', 'ASOCIADO', 1, 1, '19.403.547-0')</t>
+    <t>('Leonardo Leiva C', 'PROPIO', 0, 1, '16.166.731-5')</t>
+  </si>
+  <si>
+    <t>('ALEX MILLAR', 'ASOCIADO', 1, 1, '9.716.038-4')</t>
+  </si>
+  <si>
+    <t>('MIGUEL PEÑAHERRERA P', 'PORTEADOR', 0, 1, '28.278.056-9')</t>
+  </si>
+  <si>
+    <t>('Pablo Tudela M', 'PROPIO', 0, 1, '15.893.630-5')</t>
+  </si>
+  <si>
+    <t>('LUIS PAILLALEF P', 'PORTEADOR', 0, 1, '10.048.208-8')</t>
   </si>
   <si>
     <t>('PATRICIO PARDO V', 'PORTEADOR', 0, 1, '13.546.027-3')</t>
   </si>
   <si>
-    <t>('Nelson Gallardo R', 'PROPIO', 0, 1, '11.388.715-K')</t>
-  </si>
-  <si>
-    <t>('CRISTIAN LLANCA P', 'ASOCIADO', 1, 1, '19.143.316-5')</t>
-  </si>
-  <si>
-    <t>('DOMINGO LLANOS', 'ASOCIADO', 1, 1, '10.767.591-4')</t>
-  </si>
-  <si>
-    <t>('ANGEL FLORES H', 'ASOCIADO', 1, 1, '16.668.125-1')</t>
-  </si>
-  <si>
-    <t>('ANDY BETANCOURT H', 'PROPIO', 0, 1, '16.300.244-2')</t>
-  </si>
-  <si>
-    <t>('MAURICIO URBINA S', 'PROPIO', 0, 1, '11.630.504-6')</t>
-  </si>
-  <si>
-    <t>('CRISTIAN REAL M', 'PORTEADOR', 0, 1, '16.642.093-8')</t>
-  </si>
-  <si>
-    <t>('Pablo Tudela M', 'PROPIO', 0, 1, '15.893.630-5')</t>
-  </si>
-  <si>
-    <t>('Luis Olea V', 'PROPIO', 0, 1, '16.491.628-6')</t>
-  </si>
-  <si>
-    <t>('MAURICIO RIVAS R', 'ASOCIADO', 1, 1, '18.448.238-K')</t>
+    <t>('CARLOS OSORIO', 'ASOCIADO', 1, 1, '13.368.536-7')</t>
+  </si>
+  <si>
+    <t>('FELIPE ROJAS S', 'ASOCIADO', 1, 1, '19.756.747-3')</t>
+  </si>
+  <si>
+    <t>('Francisco Paredes A', 'PROPIO', 0, 1, '13.837.221-9')</t>
+  </si>
+  <si>
+    <t>('LEONARDO MIRANDA B', 'ASOCIADO', 1, 1, '13.547.264-6')</t>
+  </si>
+  <si>
+    <t>('DERWINS CORTEZ G', 'ASOCIADO', 1, 1, '26.536.138-2')</t>
+  </si>
+  <si>
+    <t>('FLAVIO PACHECO P', 'PROPIO', 0, 1, '27.918.005-4')</t>
   </si>
   <si>
     <t>('FELIPE RIVAS D', 'PROPIO', 0, 1, '16.517.262-0')</t>
   </si>
   <si>
-    <t>('GUILLERMO GARAY', 'ASOCIADO', 1, 1, '15.648.946-8')</t>
-  </si>
-  <si>
-    <t>('FELIPE ROJAS S', 'ASOCIADO', 1, 1, '19.756.747-3')</t>
-  </si>
-  <si>
-    <t>('JHONNY SEPULVEDA', 'ASOCIADO', 1, 1, '16.130.818-8')</t>
-  </si>
-  <si>
-    <t>('CARLOS PONCE A', 'PROPIO', 0, 1, '14.555.433-0')</t>
-  </si>
-  <si>
-    <t>('JUAN VICENCIO N', 'PROPIO', 0, 1, '15.095.552-1')</t>
-  </si>
-  <si>
-    <t>('OWEN AGUILAR G', 'ASOCIADO', 1, 1, '15.873.472-9')</t>
-  </si>
-  <si>
-    <t>('DANIEL BEJARANO H', 'PROPIO', 0, 1, '27.886.201-1')</t>
-  </si>
-  <si>
     <t>('YOSMAR PEREZ P', 'PROPIO', 0, 1, '11.257.434-4')</t>
   </si>
   <si>
-    <t>('SERGIO VEGA V', 'PROPIO', 0, 1, '18.122.272-7')</t>
-  </si>
-  <si>
-    <t>('MIGUEL PEÑAHERRERA P', 'PORTEADOR', 0, 1, '28.278.056-9')</t>
-  </si>
-  <si>
-    <t>('CARLOS OSORIO', 'ASOCIADO', 1, 1, '13.368.536-7')</t>
-  </si>
-  <si>
-    <t>('Luis Arevalo M', 'ASOCIADO', 1, 1, '16.529.122-0')</t>
-  </si>
-  <si>
-    <t>('EDUARDO ROMAN O', 'PROPIO', 0, 1, '11.946.072-7')</t>
-  </si>
-  <si>
-    <t>('Francisco Paredes A', 'PROPIO', 0, 1, '13.837.221-9')</t>
-  </si>
-  <si>
-    <t>('CARLOS AREVALO M', 'PROPIO', 0, 1, '17.149.048-0')</t>
-  </si>
-  <si>
-    <t>('FERNANDO COFRÉ T', 'PROPIO', 0, 1, '15.112.544-1')</t>
-  </si>
-  <si>
-    <t>('CRISTIAN MUÑOZ S', 'ASOCIADO', 1, 1, '13.196.333-5')</t>
-  </si>
-  <si>
-    <t>('FLAVIO PACHECO P', 'PROPIO', 0, 1, '27.918.005-4')</t>
-  </si>
-  <si>
-    <t>('GABRIEL PARRA C', 'ASOCIADO', 1, 1, '18.759.852-4')</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:54:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:55:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 12:30:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:27:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:54:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:40:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:54:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:10:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:36:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 03:52:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:20:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:28:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:26:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 12:20:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:10:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:06:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:30:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:38:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:41:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:42:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:26:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:58:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:39:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:07:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:25:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 17:20:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 03:18:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 12:52:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 12:56:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 14:06:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:31:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:19:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 16:12:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:54:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:31:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 17:04:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 03:39:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 14:00:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:21:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:20:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 16:40:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 03:00:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:48:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:08:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 16:53:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:00:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:24:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 03:06:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:01:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:24:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 12:36:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:55:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:56:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 15:48:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:04:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:20:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 07:10:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 17:22:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:20:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:58:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 07:30:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:50:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:55:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:44:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:42:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:26:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:53:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 07:16:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:37:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:20:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:40:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:31:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 02:29:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 04:46:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:00:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:25:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:28:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:44:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:14:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:14:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 22:08:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:42:33</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:02:39</t>
-  </si>
-  <si>
-    <t>2024-04-08 07:00:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 07:14:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 14:30:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:16:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:12:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:19:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:48:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:46:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:40:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:26:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:50:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:06:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 16:24:44</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:02:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:46:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:18:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 14:25:45</t>
-  </si>
-  <si>
-    <t>2024-04-08 07:27:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 12:12:21</t>
-  </si>
-  <si>
-    <t>2024-04-08 18:40:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 05:58:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 14:12:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 14:16:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 15:26:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 09:47:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 07:39:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 17:32:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:14:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 15:12:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 18:24:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:25:45</t>
-  </si>
-  <si>
-    <t>2024-04-08 15:20:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:41:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 12:24:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 18:00:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:27:28</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:08:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:36:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 18:13:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 19:14:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:44:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 17:17:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:10:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:56:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:16:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 17:08:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 20:06:28</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:47:33</t>
-  </si>
-  <si>
-    <t>2024-04-08 17:09:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 18:42:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:19:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 13:44:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 15:18:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:30:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:51:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:10:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 15:14:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:04:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:02:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:48:33</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:01:39</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:57:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:40:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 11:00:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:55:21</t>
-  </si>
-  <si>
-    <t>2024-04-08 06:06:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 19:00:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 07:45:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:48:00</t>
-  </si>
-  <si>
-    <t>2024-04-08 10:32:28</t>
-  </si>
-  <si>
-    <t>2024-04-08 08:04:00</t>
+    <t>2024-04-16 08:50:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 02:39:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 13:28:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:59:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:59:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 03:15:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 03:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:20:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:30:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:10:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 07:20:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 02:30:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:30:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 07:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 03:43:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:57:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 03:16:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 02:29:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:32:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 01:12:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:36:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:50:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 02:59:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 02:57:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 02:16:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 17:20:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 15:36:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:16:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 07:59:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:24:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 03:22:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:26:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:50:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:36:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 15:50:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:02:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:46:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 14:01:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:34:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 03:58:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:48:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:52:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 16:28:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:08:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:31:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:25:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:04:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 01:38:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:14:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 01:50:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:44:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 13:29:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 15:56:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 07:44:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:20:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:10:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 16:32:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:34:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:43:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 03:08:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 03:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:51:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:42:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:50:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 17:32:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 02:25:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:29:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:24:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:58:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:16:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 16:44:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 04:57:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:31:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:30:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:10:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:28:28</t>
+  </si>
+  <si>
+    <t>2024-04-16 14:48:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:56:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 15:58:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:41:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:34:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 07:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 13:15:28</t>
+  </si>
+  <si>
+    <t>2024-04-16 14:19:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:10:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 17:34:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 15:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:41:28</t>
+  </si>
+  <si>
+    <t>2024-04-16 20:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:02:50</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:46:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:32:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 13:45:28</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:01:19</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:52:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:01:16</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:26:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:30:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:56:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:10:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:56:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:46:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:05:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:57:31</t>
+  </si>
+  <si>
+    <t>2024-04-16 18:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 13:10:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 16:56:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:05:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:06:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:55:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:11:28</t>
+  </si>
+  <si>
+    <t>2024-04-16 14:58:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 16:42:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:54:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 13:19:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 19:37:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:19:13</t>
+  </si>
+  <si>
+    <t>2024-04-16 20:53:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 17:10:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:22:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:10:19</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:06:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 15:21:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:16:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:08:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 09:26:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:12:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 17:48:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 18:32:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:28:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 16:47:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 07:45:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:24:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:40:28</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:34:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:17:33</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:04:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 14:49:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 17:16:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 14:23:24</t>
+  </si>
+  <si>
+    <t>2024-04-16 12:35:49</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:40:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 17:52:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 05:54:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 19:04:28</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:48:33</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:06:51</t>
+  </si>
+  <si>
+    <t>2024-04-16 14:11:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 07:02:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:10:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 18:52:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:53:21</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:49:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 17:42:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 19:22:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 06:36:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 11:53:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 18:04:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 08:46:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 13:45:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 14:04:00</t>
+  </si>
+  <si>
+    <t>2024-04-16 10:04:00</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1108,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1013,19 +1136,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>97023</v>
+        <v>97243</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>45390.4125</v>
+        <v>45398.36805555555</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="F2" s="3">
         <v>0.05555555555555555</v>
@@ -1033,139 +1156,139 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>96904</v>
+        <v>97440</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>45390.20486111111</v>
+        <v>45398.11041666667</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="F3" s="3">
-        <v>0.3465277777777778</v>
+        <v>0.2843611111111111</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>96586</v>
+        <v>97469</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>45390.52083333334</v>
+        <v>45398.56111111111</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="F4" s="3">
-        <v>0.4013888888888889</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>96736</v>
+        <v>97194</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2">
-        <v>45390.10208333333</v>
+        <v>45398.20763888889</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="F5" s="3">
-        <v>0.3441388888888889</v>
+        <v>0.33125</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>96897</v>
+        <v>97224</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>45390.12083333333</v>
+        <v>45398.37430555555</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="F6" s="3">
-        <v>0.2976805555555556</v>
+        <v>0.2909722222222222</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>97000</v>
+        <v>97320</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2">
-        <v>45390.23611111111</v>
+        <v>45398.13541666666</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="F7" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.2680555555555555</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>96871</v>
+        <v>97423</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>45390.24583333333</v>
+        <v>45398.125</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="F8" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3569444444444445</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>96924</v>
+        <v>97521</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
-        <v>45390.54861111111</v>
+        <v>45398.26388888889</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="F9" s="3">
         <v>0.05555555555555555</v>
@@ -1173,39 +1296,39 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>97041</v>
+        <v>97149</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
-        <v>45390.35833333333</v>
+        <v>45398.1875</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="F10" s="3">
-        <v>0.1111111111111111</v>
+        <v>0.3649166666666667</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>97066</v>
+        <v>97238</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
-        <v>45390.16111111111</v>
+        <v>45398.21527777778</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="F11" s="3">
         <v>0.05555555555555555</v>
@@ -1213,19 +1336,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>96622</v>
+        <v>97239</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
-        <v>45390.18055555555</v>
+        <v>45398.30555555555</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="F12" s="3">
         <v>0.2909722222222222</v>
@@ -1233,339 +1356,339 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>97128</v>
+        <v>96975</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2">
-        <v>45390.18611111111</v>
+        <v>45398.10416666666</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="F13" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>97012</v>
+        <v>97105</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2">
-        <v>45390.39305555556</v>
+        <v>45398.39583333334</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="F14" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3361111111111111</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>97064</v>
+        <v>97490</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="2">
-        <v>45390.51388888889</v>
+        <v>45398.29166666666</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="F15" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>97016</v>
+        <v>97327</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="2">
-        <v>45390.25694444445</v>
+        <v>45398.10416666666</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="F16" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.4246388888888889</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>97053</v>
+        <v>97561</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="2">
-        <v>45390.17083333333</v>
+        <v>45398.16666666666</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
       <c r="F17" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>96263</v>
+        <v>96873</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="2">
-        <v>45390.1875</v>
+        <v>45398.41666666666</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="F18" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>96039</v>
+        <v>97061</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="2">
-        <v>45390.19305555556</v>
+        <v>45398.15486111111</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="E19" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="F19" s="3">
-        <v>0.1444444444444444</v>
+        <v>0.3054444444444445</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>96488</v>
+        <v>97212</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2">
-        <v>45390.36180555556</v>
+        <v>45398.28958333333</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="F20" s="3">
-        <v>0.3220416666666667</v>
+        <v>0.1590277777777778</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>96935</v>
+        <v>96957</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="2">
-        <v>45390.19583333333</v>
+        <v>45398.13611111111</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F21" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3027777777777778</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>96998</v>
+        <v>97146</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2">
-        <v>45390.18472222222</v>
+        <v>45398.20833333334</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="F22" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3649166666666667</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>97006</v>
+        <v>97096</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23" s="2">
-        <v>45390.29027777778</v>
+        <v>45398.10347222222</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="E23" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="F23" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3974444444444444</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>96820</v>
+        <v>97500</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2">
-        <v>45390.27708333333</v>
+        <v>45398.23055555556</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="F24" s="3">
-        <v>0.3241388888888889</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>97022</v>
+        <v>94685</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2">
-        <v>45390.25486111111</v>
+        <v>45398.125</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="F25" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3758888888888889</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>96910</v>
+        <v>97397</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C26" s="2">
-        <v>45390.18402777778</v>
+        <v>45398.27777777778</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="F26" s="3">
-        <v>0.3245555555555555</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>97052</v>
+        <v>97245</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C27" s="2">
-        <v>45390.72222222222</v>
+        <v>45398.05</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="E27" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="F27" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.4263888888888889</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>97082</v>
+        <v>97007</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2">
-        <v>45390.1375</v>
+        <v>45398.13611111111</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="F28" s="3">
-        <v>0.1111111111111111</v>
+        <v>0.3013888888888889</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>96906</v>
+        <v>97502</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2">
-        <v>45390.53611111111</v>
+        <v>45398.19166666667</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="E29" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="F29" s="3">
         <v>0.05555555555555555</v>
@@ -1573,39 +1696,39 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>96905</v>
+        <v>97492</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C30" s="2">
-        <v>45390.53888888889</v>
+        <v>45398.125</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="F30" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>96980</v>
+        <v>97226</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C31" s="2">
-        <v>45390.5875</v>
+        <v>45398.20138888889</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="F31" s="3">
         <v>0.05555555555555555</v>
@@ -1613,119 +1736,119 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>96645</v>
+        <v>97193</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C32" s="2">
-        <v>45390.10486111111</v>
+        <v>45398.12430555555</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="F32" s="3">
-        <v>0.3027777777777778</v>
+        <v>0.33125</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>97002</v>
+        <v>97491</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2">
-        <v>45390.26319444444</v>
+        <v>45398.125</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="F33" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>97092</v>
+        <v>97213</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2">
-        <v>45390.675</v>
+        <v>45398.12291666667</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="F34" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.1590277777777778</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>97046</v>
+        <v>97130</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C35" s="2">
-        <v>45390.2875</v>
+        <v>45398.09444444445</v>
       </c>
       <c r="D35" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="F35" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3256944444444445</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>96596</v>
+        <v>97305</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C36" s="2">
-        <v>45390.27152777778</v>
+        <v>45398.10416666666</v>
       </c>
       <c r="D36" t="s">
         <v>83</v>
       </c>
       <c r="E36" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="F36" s="3">
-        <v>0.3618055555555555</v>
+        <v>0.3107777777777778</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>96932</v>
+        <v>97356</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C37" s="2">
-        <v>45390.71111111111</v>
+        <v>45398.72222222222</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="F37" s="3">
         <v>0.05555555555555555</v>
@@ -1733,39 +1856,39 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>96828</v>
+        <v>96697</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C38" s="2">
-        <v>45390.15208333333</v>
+        <v>45398.1875</v>
       </c>
       <c r="D38" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="F38" s="3">
-        <v>0.3241388888888889</v>
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>97042</v>
+        <v>97498</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C39" s="2">
-        <v>45390.58333333334</v>
+        <v>45398.65</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="F39" s="3">
         <v>0.05555555555555555</v>
@@ -1773,279 +1896,279 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40">
-        <v>97127</v>
+        <v>97131</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C40" s="2">
-        <v>45390.22291666667</v>
+        <v>45398.17777777778</v>
       </c>
       <c r="D40" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="E40" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="F40" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3256944444444445</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
-        <v>96621</v>
+        <v>97496</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C41" s="2">
-        <v>45390.22222222222</v>
+        <v>45398.21527777778</v>
       </c>
       <c r="D41" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F41" s="3">
-        <v>0.2944444444444445</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>96402</v>
+        <v>97479</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C42" s="2">
-        <v>45390.69444444445</v>
+        <v>45398.1875</v>
       </c>
       <c r="D42" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E42" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="F42" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3166666666666667</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>96950</v>
+        <v>97406</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C43" s="2">
-        <v>45390.125</v>
+        <v>45398.16666666666</v>
       </c>
       <c r="D43" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E43" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="F43" s="3">
-        <v>0.31075</v>
+        <v>0.3298611111111111</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>97019</v>
+        <v>97186</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="C44" s="2">
-        <v>45390.49166666667</v>
+        <v>45398.1875</v>
       </c>
       <c r="D44" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="F44" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.1538055555555556</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>96038</v>
+        <v>97223</v>
       </c>
       <c r="B45" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C45" s="2">
-        <v>45390.33888888889</v>
+        <v>45398.33263888889</v>
       </c>
       <c r="D45" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="E45" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="F45" s="3">
-        <v>0.1444444444444444</v>
+        <v>0.2909722222222222</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>96035</v>
+        <v>97336</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C46" s="2">
-        <v>45390.19305555556</v>
+        <v>45398.35</v>
       </c>
       <c r="D46" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="E46" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="F46" s="3">
-        <v>0.1444444444444444</v>
+        <v>0.3458333333333333</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>97057</v>
+        <v>97250</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C47" s="2">
-        <v>45390.70347222222</v>
+        <v>45398.14027777778</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="E47" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="F47" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3138888888888889</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>96824</v>
+        <v>97229</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C48" s="2">
-        <v>45390.41666666666</v>
+        <v>45398.26388888889</v>
       </c>
       <c r="D48" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E48" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="F48" s="3">
-        <v>0.3847222222222222</v>
+        <v>0.2909722222222222</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49">
-        <v>96936</v>
+        <v>97499</v>
       </c>
       <c r="B49" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C49" s="2">
-        <v>45390.39166666667</v>
+        <v>45398.18472222222</v>
       </c>
       <c r="D49" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="E49" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="F49" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.6326388888888889</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50">
-        <v>97081</v>
+        <v>95309</v>
       </c>
       <c r="B50" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C50" s="2">
-        <v>45390.12916666667</v>
+        <v>45398.16666666666</v>
       </c>
       <c r="D50" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>198</v>
       </c>
       <c r="F50" s="3">
-        <v>0.1111111111111111</v>
+        <v>0.2216805555555556</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>96729</v>
+        <v>97562</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C51" s="2">
-        <v>45390.41736111111</v>
+        <v>45398.24305555555</v>
       </c>
       <c r="D51" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="E51" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="F51" s="3">
-        <v>0.3027777777777778</v>
+        <v>0.6270833333333333</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
-        <v>97126</v>
+        <v>97231</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C52" s="2">
-        <v>45390.1</v>
+        <v>45398.4</v>
       </c>
       <c r="D52" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="E52" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="F52" s="3">
-        <v>0.3652777777777778</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>97089</v>
+        <v>97190</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C53" s="2">
-        <v>45390.525</v>
+        <v>45398.65972222222</v>
       </c>
       <c r="D53" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="E53" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="F53" s="3">
         <v>0.05555555555555555</v>
@@ -2053,139 +2176,139 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>96909</v>
+        <v>96665</v>
       </c>
       <c r="B54" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C54" s="2">
-        <v>45390.12152777778</v>
+        <v>45398.16805555556</v>
       </c>
       <c r="D54" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="E54" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="F54" s="3">
-        <v>0.3465277777777778</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
-        <v>96903</v>
+        <v>97097</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="C55" s="2">
-        <v>45390.49722222222</v>
+        <v>45398.10416666666</v>
       </c>
       <c r="D55" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="E55" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="F55" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.403</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56">
-        <v>97098</v>
+        <v>97493</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C56" s="2">
-        <v>45390.65833333333</v>
+        <v>45398.29166666666</v>
       </c>
       <c r="D56" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="E56" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F56" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3611111111111111</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
-        <v>96801</v>
+        <v>97191</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="2">
-        <v>45390.54444444444</v>
+        <v>45398.19861111111</v>
       </c>
       <c r="D57" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="E57" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="F57" s="3">
-        <v>0.2933888888888889</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>96737</v>
+        <v>97289</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C58" s="2">
-        <v>45390.09722222222</v>
+        <v>45398.58402777778</v>
       </c>
       <c r="D58" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E58" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="F58" s="3">
-        <v>0.3524722222222222</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>96288</v>
+        <v>97235</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C59" s="2">
-        <v>45390.29861111111</v>
+        <v>45398.39861111111</v>
       </c>
       <c r="D59" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="E59" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="F59" s="3">
-        <v>0.4159722222222222</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
-        <v>97091</v>
+        <v>97438</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C60" s="2">
-        <v>45390.72361111111</v>
+        <v>45398.36111111111</v>
       </c>
       <c r="D60" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E60" t="s">
-        <v>181</v>
+        <v>87</v>
       </c>
       <c r="F60" s="3">
         <v>0.05555555555555555</v>
@@ -2193,39 +2316,39 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61">
-        <v>96623</v>
+        <v>97308</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C61" s="2">
-        <v>45390.26388888889</v>
+        <v>45398.16527777778</v>
       </c>
       <c r="D61" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E61" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="F61" s="3">
-        <v>0.2909722222222222</v>
+        <v>0.3458333333333333</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
-        <v>96988</v>
+        <v>97468</v>
       </c>
       <c r="B62" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C62" s="2">
-        <v>45390.19305555556</v>
+        <v>45398.40833333333</v>
       </c>
       <c r="D62" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="E62" t="s">
-        <v>152</v>
+        <v>206</v>
       </c>
       <c r="F62" s="3">
         <v>0.05555555555555555</v>
@@ -2233,39 +2356,39 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
-        <v>97073</v>
+        <v>97418</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C63" s="2">
-        <v>45390.125</v>
+        <v>45398.125</v>
       </c>
       <c r="D63" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E63" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="F63" s="3">
-        <v>0.4472222222222222</v>
+        <v>0.2680555555555555</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64">
-        <v>96911</v>
+        <v>97398</v>
       </c>
       <c r="B64" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C64" s="2">
-        <v>45390.19305555556</v>
+        <v>45398.41111111111</v>
       </c>
       <c r="D64" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="E64" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="F64" s="3">
         <v>0.05555555555555555</v>
@@ -2273,19 +2396,19 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65">
-        <v>97013</v>
+        <v>97227</v>
       </c>
       <c r="B65" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="C65" s="2">
-        <v>45390.58194444444</v>
+        <v>45398.68611111111</v>
       </c>
       <c r="D65" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E65" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="F65" s="3">
         <v>0.05555555555555555</v>
@@ -2293,139 +2416,139 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66">
-        <v>97044</v>
+        <v>97151</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C66" s="2">
-        <v>45390.3125</v>
+        <v>45398.45833333334</v>
       </c>
       <c r="D66" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E66" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="F66" s="3">
-        <v>0.1666666666666667</v>
+        <v>0.3138888888888889</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67">
-        <v>96979</v>
+        <v>96666</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C67" s="2">
-        <v>45390.125</v>
+        <v>45398.38055555556</v>
       </c>
       <c r="D67" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="E67" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="F67" s="3">
-        <v>0.3270833333333333</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68">
-        <v>96331</v>
+        <v>97290</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C68" s="2">
-        <v>45390.28472222222</v>
+        <v>45398.39652777778</v>
       </c>
       <c r="D68" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="E68" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="F68" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3027777777777778</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69">
-        <v>96907</v>
+        <v>97474</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C69" s="2">
-        <v>45390.28819444445</v>
+        <v>45398.26736111111</v>
       </c>
       <c r="D69" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="E69" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="F69" s="3">
-        <v>0.3465277777777778</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70">
-        <v>96949</v>
+        <v>97399</v>
       </c>
       <c r="B70" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C70" s="2">
-        <v>45390.125</v>
+        <v>45398.37777777778</v>
       </c>
       <c r="D70" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="E70" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="F70" s="3">
-        <v>0.31075</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71">
-        <v>97021</v>
+        <v>96349</v>
       </c>
       <c r="B71" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C71" s="2">
-        <v>45390.4125</v>
+        <v>45398.06805555556</v>
       </c>
       <c r="D71" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="E71" t="s">
-        <v>127</v>
+        <v>215</v>
       </c>
       <c r="F71" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.2933888888888889</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72">
-        <v>97020</v>
+        <v>96667</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C72" s="2">
-        <v>45390.40555555555</v>
+        <v>45398.38472222222</v>
       </c>
       <c r="D72" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="E72" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="F72" s="3">
         <v>0.05555555555555555</v>
@@ -2433,79 +2556,79 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73">
-        <v>97051</v>
+        <v>97328</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C73" s="2">
-        <v>45390.40416666667</v>
+        <v>45398.07638888889</v>
       </c>
       <c r="D73" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="E73" t="s">
-        <v>190</v>
+        <v>217</v>
       </c>
       <c r="F73" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3524722222222222</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74">
-        <v>96748</v>
+        <v>97501</v>
       </c>
       <c r="B74" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C74" s="2">
-        <v>45390.10138888889</v>
+        <v>45398.23611111111</v>
       </c>
       <c r="D74" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E74" t="s">
-        <v>191</v>
+        <v>85</v>
       </c>
       <c r="F74" s="3">
-        <v>0.349</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75">
-        <v>97015</v>
+        <v>97230</v>
       </c>
       <c r="B75" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C75" s="2">
-        <v>45390.12013888889</v>
+        <v>45398.19722222222</v>
       </c>
       <c r="D75" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="E75" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="F75" s="3">
-        <v>0.2976805555555556</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76">
-        <v>97067</v>
+        <v>97396</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C76" s="2">
-        <v>45390.30277777778</v>
+        <v>45398.56180555555</v>
       </c>
       <c r="D76" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="E76" t="s">
-        <v>57</v>
+        <v>219</v>
       </c>
       <c r="F76" s="3">
         <v>0.05555555555555555</v>
@@ -2513,19 +2636,19 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77">
-        <v>96982</v>
+        <v>97241</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="C77" s="2">
-        <v>45390.23402777778</v>
+        <v>45398.66388888889</v>
       </c>
       <c r="D77" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="E77" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="F77" s="3">
         <v>0.05555555555555555</v>
@@ -2533,59 +2656,59 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78">
-        <v>96908</v>
+        <v>96810</v>
       </c>
       <c r="B78" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C78" s="2">
-        <v>45390.38888888889</v>
+        <v>45398.32222222222</v>
       </c>
       <c r="D78" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="E78" t="s">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c r="F78" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.2773611111111111</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79">
-        <v>96739</v>
+        <v>97391</v>
       </c>
       <c r="B79" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C79" s="2">
-        <v>45390.09722222222</v>
+        <v>45398.1875</v>
       </c>
       <c r="D79" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E79" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
       <c r="F79" s="3">
-        <v>0.3524722222222222</v>
+        <v>0.337375</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80">
-        <v>97054</v>
+        <v>97331</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C80" s="2">
-        <v>45390.40277777778</v>
+        <v>45398.19722222222</v>
       </c>
       <c r="D80" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E80" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
       <c r="F80" s="3">
         <v>0.05555555555555555</v>
@@ -2593,59 +2716,59 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
-        <v>97014</v>
+        <v>97439</v>
       </c>
       <c r="B81" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C81" s="2">
-        <v>45390.18819444445</v>
+        <v>45398.40277777778</v>
       </c>
       <c r="D81" t="s">
+        <v>133</v>
+      </c>
+      <c r="E81" t="s">
         <v>120</v>
       </c>
-      <c r="E81" t="s">
-        <v>123</v>
-      </c>
       <c r="F81" s="3">
-        <v>0.1868055555555556</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82">
-        <v>96545</v>
+        <v>97303</v>
       </c>
       <c r="B82" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C82" s="2">
-        <v>45390.10347222222</v>
+        <v>45398.38888888889</v>
       </c>
       <c r="D82" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="E82" t="s">
-        <v>196</v>
+        <v>223</v>
       </c>
       <c r="F82" s="3">
-        <v>0.2683055555555555</v>
+        <v>0.05555555555555555</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83">
-        <v>96983</v>
+        <v>97390</v>
       </c>
       <c r="B83" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C83" s="2">
-        <v>45390.19861111111</v>
+        <v>45398.38194444445</v>
       </c>
       <c r="D83" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="E83" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="F83" s="3">
         <v>0.05555555555555555</v>
@@ -2653,39 +2776,39 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84">
-        <v>96634</v>
+        <v>97560</v>
       </c>
       <c r="B84" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C84" s="2">
-        <v>45390.375</v>
+        <v>45398.33333333334</v>
       </c>
       <c r="D84" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="E84" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="F84" s="3">
-        <v>0.4166666666666667</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85">
-        <v>97018</v>
+        <v>97494</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="C85" s="2">
-        <v>45390.26736111111</v>
+        <v>45398.68888888889</v>
       </c>
       <c r="D85" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="E85" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="F85" s="3">
         <v>0.05555555555555555</v>
@@ -2693,19 +2816,19 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
-        <v>96870</v>
+        <v>97503</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="C86" s="2">
-        <v>45390.39444444444</v>
+        <v>45398.19027777778</v>
       </c>
       <c r="D86" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="E86" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="F86" s="3">
         <v>0.05555555555555555</v>
@@ -2713,62 +2836,382 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87">
-        <v>96948</v>
+        <v>97318</v>
       </c>
       <c r="B87" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C87" s="2">
-        <v>45390.15208333333</v>
+        <v>45398.48819444444</v>
       </c>
       <c r="D87" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="E87" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="F87" s="3">
-        <v>0.2871388888888889</v>
+        <v>0.3065833333333333</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88">
-        <v>96922</v>
+        <v>97242</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="C88" s="2">
-        <v>45390.1875</v>
+        <v>45398.13055555556</v>
       </c>
       <c r="D88" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="E88" t="s">
-        <v>142</v>
+        <v>227</v>
       </c>
       <c r="F88" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.3198333333333333</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
-        <v>96994</v>
+        <v>97317</v>
       </c>
       <c r="B89" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C89" s="2">
-        <v>45390.28055555555</v>
+        <v>45398.15277777778</v>
       </c>
       <c r="D89" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="E89" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="F89" s="3">
-        <v>0.05555555555555555</v>
+        <v>0.2686527777777777</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90">
+        <v>97225</v>
+      </c>
+      <c r="B90" t="s">
+        <v>69</v>
+      </c>
+      <c r="C90" s="2">
+        <v>45398.19722222222</v>
+      </c>
+      <c r="D90" t="s">
+        <v>129</v>
+      </c>
+      <c r="E90" t="s">
+        <v>139</v>
+      </c>
+      <c r="F90" s="3">
+        <v>0.2909722222222222</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91">
+        <v>97192</v>
+      </c>
+      <c r="B91" t="s">
+        <v>39</v>
+      </c>
+      <c r="C91" s="2">
+        <v>45398.53541666667</v>
+      </c>
+      <c r="D91" t="s">
+        <v>142</v>
+      </c>
+      <c r="E91" t="s">
+        <v>229</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92">
+        <v>97150</v>
+      </c>
+      <c r="B92" t="s">
+        <v>60</v>
+      </c>
+      <c r="C92" s="2">
+        <v>45398.2375</v>
+      </c>
+      <c r="D92" t="s">
+        <v>143</v>
+      </c>
+      <c r="E92" t="s">
+        <v>230</v>
+      </c>
+      <c r="F92" s="3">
+        <v>0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93">
+        <v>97298</v>
+      </c>
+      <c r="B93" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" s="2">
+        <v>45398.28472222222</v>
+      </c>
+      <c r="D93" t="s">
+        <v>144</v>
+      </c>
+      <c r="E93" t="s">
+        <v>231</v>
+      </c>
+      <c r="F93" s="3">
+        <v>0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94">
+        <v>97330</v>
+      </c>
+      <c r="B94" t="s">
+        <v>36</v>
+      </c>
+      <c r="C94" s="2">
+        <v>45398.73055555556</v>
+      </c>
+      <c r="D94" t="s">
+        <v>145</v>
+      </c>
+      <c r="E94" t="s">
+        <v>232</v>
+      </c>
+      <c r="F94" s="3">
+        <v>0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95">
+        <v>96882</v>
+      </c>
+      <c r="B95" t="s">
+        <v>70</v>
+      </c>
+      <c r="C95" s="2">
+        <v>45398.10069444445</v>
+      </c>
+      <c r="D95" t="s">
+        <v>146</v>
+      </c>
+      <c r="E95" t="s">
+        <v>233</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0.2696944444444444</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <v>97309</v>
+      </c>
+      <c r="B96" t="s">
+        <v>41</v>
+      </c>
+      <c r="C96" s="2">
+        <v>45398.39513888889</v>
+      </c>
+      <c r="D96" t="s">
+        <v>147</v>
+      </c>
+      <c r="E96" t="s">
+        <v>234</v>
+      </c>
+      <c r="F96" s="3">
+        <v>0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
+        <v>97335</v>
+      </c>
+      <c r="B97" t="s">
+        <v>70</v>
+      </c>
+      <c r="C97" s="2">
+        <v>45398.39166666667</v>
+      </c>
+      <c r="D97" t="s">
+        <v>148</v>
+      </c>
+      <c r="E97" t="s">
+        <v>235</v>
+      </c>
+      <c r="F97" s="3">
+        <v>0.3458333333333333</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <v>97294</v>
+      </c>
+      <c r="B98" t="s">
+        <v>67</v>
+      </c>
+      <c r="C98" s="2">
+        <v>45398.29027777778</v>
+      </c>
+      <c r="D98" t="s">
+        <v>149</v>
+      </c>
+      <c r="E98" t="s">
+        <v>236</v>
+      </c>
+      <c r="F98" s="3">
+        <v>0.5166666666666667</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <v>97495</v>
+      </c>
+      <c r="B99" t="s">
+        <v>21</v>
+      </c>
+      <c r="C99" s="2">
+        <v>45398.21944444445</v>
+      </c>
+      <c r="D99" t="s">
+        <v>150</v>
+      </c>
+      <c r="E99" t="s">
+        <v>237</v>
+      </c>
+      <c r="F99" s="3">
+        <v>0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <v>97293</v>
+      </c>
+      <c r="B100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C100" s="2">
+        <v>45398.125</v>
+      </c>
+      <c r="D100" t="s">
+        <v>78</v>
+      </c>
+      <c r="E100" t="s">
+        <v>238</v>
+      </c>
+      <c r="F100" s="3">
+        <v>0.3701388888888889</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <v>97497</v>
+      </c>
+      <c r="B101" t="s">
+        <v>33</v>
+      </c>
+      <c r="C101" s="2">
+        <v>45398.69722222222</v>
+      </c>
+      <c r="D101" t="s">
+        <v>151</v>
+      </c>
+      <c r="E101" t="s">
+        <v>239</v>
+      </c>
+      <c r="F101" s="3">
+        <v>0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102">
+        <v>97210</v>
+      </c>
+      <c r="B102" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" s="2">
+        <v>45398.20625</v>
+      </c>
+      <c r="D102" t="s">
+        <v>152</v>
+      </c>
+      <c r="E102" t="s">
+        <v>240</v>
+      </c>
+      <c r="F102" s="3">
+        <v>0.1590277777777778</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103">
+        <v>97004</v>
+      </c>
+      <c r="B103" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" s="2">
+        <v>45398.27152777778</v>
+      </c>
+      <c r="D103" t="s">
+        <v>153</v>
+      </c>
+      <c r="E103" t="s">
+        <v>241</v>
+      </c>
+      <c r="F103" s="3">
+        <v>0.3013888888888889</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104">
+        <v>97139</v>
+      </c>
+      <c r="B104" t="s">
+        <v>14</v>
+      </c>
+      <c r="C104" s="2">
+        <v>45398.27083333334</v>
+      </c>
+      <c r="D104" t="s">
+        <v>154</v>
+      </c>
+      <c r="E104" t="s">
+        <v>242</v>
+      </c>
+      <c r="F104" s="3">
+        <v>0.3152777777777778</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105">
+        <v>97480</v>
+      </c>
+      <c r="B105" t="s">
+        <v>71</v>
+      </c>
+      <c r="C105" s="2">
+        <v>45398.10416666666</v>
+      </c>
+      <c r="D105" t="s">
+        <v>83</v>
+      </c>
+      <c r="E105" t="s">
+        <v>243</v>
+      </c>
+      <c r="F105" s="3">
+        <v>0.3152777777777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>